<commit_message>
Planilha com dados dos gráficos
Fiz até o último gráfico da página 177
</commit_message>
<xml_diff>
--- a/Dados - JetStar.xlsx
+++ b/Dados - JetStar.xlsx
@@ -4,13 +4,17 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="alpha_zero_mach" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="cl_mach" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="cd_mach" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="cl_alpha_mach" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="cd_alpha_mach" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="cm_alpha_mach" sheetId="6" r:id="rId9"/>
-    <sheet state="visible" name="cm_alphadot_mach" sheetId="7" r:id="rId10"/>
-    <sheet state="visible" name="cm_q_mach" sheetId="8" r:id="rId11"/>
+    <sheet state="visible" name="CL_mach" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="CD_mach" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="CL_alpha_mach" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="CD_alpha_mach" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="Cm_alpha_mach" sheetId="6" r:id="rId9"/>
+    <sheet state="visible" name="Cm_alphadot_mach" sheetId="7" r:id="rId10"/>
+    <sheet state="visible" name="Cm_q_mach" sheetId="8" r:id="rId11"/>
+    <sheet state="visible" name="CD_M_mach" sheetId="9" r:id="rId12"/>
+    <sheet state="visible" name="CM_M_mach" sheetId="10" r:id="rId13"/>
+    <sheet state="visible" name="CL_delta_e" sheetId="11" r:id="rId14"/>
+    <sheet state="visible" name="Cm_delta_e" sheetId="12" r:id="rId15"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -18,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="18">
   <si>
     <t>mach</t>
   </si>
@@ -41,25 +45,37 @@
     <t>40kft</t>
   </si>
   <si>
-    <t>cl</t>
+    <t>CL</t>
   </si>
   <si>
-    <t>cd</t>
+    <t>CD</t>
   </si>
   <si>
-    <t>cl_alpha</t>
+    <t>CL_alpha</t>
   </si>
   <si>
-    <t>cd_alpha</t>
+    <t>CD_alpha</t>
   </si>
   <si>
-    <t>cm_alpha</t>
+    <t>Cm_alpha</t>
   </si>
   <si>
-    <t>cm_alphadot</t>
+    <t>Cm_alphadot</t>
   </si>
   <si>
-    <t>cm_q</t>
+    <t>Cm_q</t>
+  </si>
+  <si>
+    <t>CD_M</t>
+  </si>
+  <si>
+    <t>CM_M</t>
+  </si>
+  <si>
+    <t>CL_delta_e</t>
+  </si>
+  <si>
+    <t>Cm_delta_e</t>
   </si>
 </sst>
 </file>
@@ -105,8 +121,11 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -115,9 +134,6 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -143,6 +159,18 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
@@ -168,6 +196,10 @@
 </file>
 
 <file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -520,6 +552,471 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="6">
+        <v>0.232592592592592</v>
+      </c>
+      <c r="B2" s="2">
+        <v>-0.0643916913946587</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6">
+        <v>0.402962962962962</v>
+      </c>
+      <c r="B3" s="2">
+        <v>-0.0658753709198813</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="6">
+        <v>0.525925925925925</v>
+      </c>
+      <c r="B4" s="2">
+        <v>-0.0213649851632047</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="6">
+        <v>0.351111111111111</v>
+      </c>
+      <c r="B5" s="2">
+        <v>-0.0762611275964391</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="6">
+        <v>0.548148148148148</v>
+      </c>
+      <c r="B6" s="2">
+        <v>-0.0080118694362018</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="6">
+        <v>0.749629629629629</v>
+      </c>
+      <c r="B7" s="2">
+        <v>-0.0881305637982196</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="6">
+        <v>0.502222222222222</v>
+      </c>
+      <c r="B8" s="2">
+        <v>8.90207715133525E-4</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="1">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="6">
+        <v>0.648888888888889</v>
+      </c>
+      <c r="B9" s="2">
+        <v>-0.00652818991097924</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="1">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="6">
+        <v>0.801481481481481</v>
+      </c>
+      <c r="B10" s="2">
+        <v>-0.61186943620178</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="1">
+        <v>10.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="6">
+        <v>0.226829268292682</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.396296296296296</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6">
+        <v>0.398780487804878</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.398765432098765</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="6">
+        <v>0.523170731707317</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.402469135802469</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="6">
+        <v>0.347560975609756</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.39753086419753</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="6">
+        <v>0.551219512195122</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.403703703703703</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="6">
+        <v>0.746341463414634</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.424691358024691</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="6">
+        <v>0.49390243902439</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.404938271604938</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="1">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="6">
+        <v>0.646341463414634</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.414814814814814</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="1">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="6">
+        <v>0.796341463414634</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.439506172839506</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="1">
+        <v>10.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="6">
+        <v>0.230882352941176</v>
+      </c>
+      <c r="B2" s="2">
+        <v>-0.81267217630854</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6">
+        <v>0.400735294117647</v>
+      </c>
+      <c r="B3" s="2">
+        <v>-0.817079889807162</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="6">
+        <v>0.526470588235294</v>
+      </c>
+      <c r="B4" s="2">
+        <v>-0.828099173553719</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="6">
+        <v>0.347794117647058</v>
+      </c>
+      <c r="B5" s="2">
+        <v>-0.81267217630854</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="6">
+        <v>0.555147058823529</v>
+      </c>
+      <c r="B6" s="2">
+        <v>-0.83030303030303</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="6">
+        <v>0.749264705882353</v>
+      </c>
+      <c r="B7" s="2">
+        <v>-0.865564738292011</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="B8" s="2">
+        <v>-0.819283746556474</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="1">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="6">
+        <v>0.65</v>
+      </c>
+      <c r="B9" s="2">
+        <v>-0.839118457300275</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="1">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="6">
+        <v>0.797794117647059</v>
+      </c>
+      <c r="B10" s="2">
+        <v>-0.883195592286501</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="1">
+        <v>10.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
@@ -534,7 +1031,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -545,10 +1042,10 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3">
+      <c r="A2" s="4">
         <v>0.257142857142857</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="4">
         <v>0.863586277030177</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -557,13 +1054,13 @@
       <c r="D2" s="1">
         <v>2.0</v>
       </c>
-      <c r="F2" s="4"/>
+      <c r="F2" s="5"/>
     </row>
     <row r="3">
-      <c r="A3" s="3">
+      <c r="A3" s="4">
         <v>0.498412698412698</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="4">
         <v>0.296031264063913</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -572,13 +1069,13 @@
       <c r="D3" s="1">
         <v>3.0</v>
       </c>
-      <c r="F3" s="4"/>
+      <c r="F3" s="5"/>
     </row>
     <row r="4">
-      <c r="A4" s="3">
+      <c r="A4" s="4">
         <v>0.615873015873015</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="4">
         <v>0.170798509501005</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -587,13 +1084,13 @@
       <c r="D4" s="1">
         <v>4.0</v>
       </c>
-      <c r="F4" s="4"/>
+      <c r="F4" s="5"/>
     </row>
     <row r="5">
-      <c r="A5" s="3">
+      <c r="A5" s="4">
         <v>0.434920634920634</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="4">
         <v>0.832496019421891</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -602,13 +1099,13 @@
       <c r="D5" s="1">
         <v>5.0</v>
       </c>
-      <c r="F5" s="4"/>
+      <c r="F5" s="5"/>
     </row>
     <row r="6">
-      <c r="A6" s="3">
+      <c r="A6" s="4">
         <v>0.628571428571428</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="4">
         <v>0.345315887833959</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -617,13 +1114,13 @@
       <c r="D6" s="1">
         <v>6.0</v>
       </c>
-      <c r="F6" s="4"/>
+      <c r="F6" s="5"/>
     </row>
     <row r="7">
-      <c r="A7" s="3">
+      <c r="A7" s="4">
         <v>0.768253968253968</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="4">
         <v>0.183793949452403</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -632,13 +1129,13 @@
       <c r="D7" s="1">
         <v>7.0</v>
       </c>
-      <c r="F7" s="4"/>
+      <c r="F7" s="5"/>
     </row>
     <row r="8">
-      <c r="A8" s="3">
+      <c r="A8" s="4">
         <v>0.587301587301587</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="4">
         <v>1.01477422272906</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -647,13 +1144,13 @@
       <c r="D8" s="1">
         <v>8.0</v>
       </c>
-      <c r="F8" s="4"/>
+      <c r="F8" s="5"/>
     </row>
     <row r="9">
-      <c r="A9" s="3">
+      <c r="A9" s="4">
         <v>0.707936507936508</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="4">
         <v>0.594135291750357</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -662,13 +1159,13 @@
       <c r="D9" s="1">
         <v>9.0</v>
       </c>
-      <c r="F9" s="4"/>
+      <c r="F9" s="5"/>
     </row>
     <row r="10">
-      <c r="A10" s="3">
+      <c r="A10" s="4">
         <v>0.793650793650793</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="4">
         <v>0.402805638680146</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -677,7 +1174,7 @@
       <c r="D10" s="1">
         <v>10.0</v>
       </c>
-      <c r="F10" s="4"/>
+      <c r="F10" s="5"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:B10 F4:F12">
@@ -703,7 +1200,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -858,7 +1355,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -869,10 +1366,10 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="6">
+      <c r="A2" s="2">
         <v>0.231003039513677</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="2">
         <v>5.05504587155963</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -883,10 +1380,10 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="6">
+      <c r="A3" s="2">
         <v>0.400607902735562</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="2">
         <v>5.14678899082568</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -897,10 +1394,10 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="6">
+      <c r="A4" s="2">
         <v>0.528267477203647</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="2">
         <v>5.25688073394495</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -911,10 +1408,10 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="6">
+      <c r="A5" s="2">
         <v>0.349544072948328</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="2">
         <v>5.16513761467889</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -925,10 +1422,10 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="6">
+      <c r="A6" s="2">
         <v>0.551975683890577</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="2">
         <v>5.33027522935779</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -939,10 +1436,10 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="6">
+      <c r="A7" s="2">
         <v>0.750759878419453</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="2">
         <v>5.93577981651376</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -953,10 +1450,10 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="6">
+      <c r="A8" s="2">
         <v>0.497264437689969</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="2">
         <v>5.23853211009174</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -967,10 +1464,10 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="6">
+      <c r="A9" s="2">
         <v>0.650455927051671</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="2">
         <v>5.47706422018348</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -981,10 +1478,10 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="6">
+      <c r="A10" s="2">
         <v>0.798176291793313</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="2">
         <v>6.3394495412844</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -1013,7 +1510,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1024,10 +1521,10 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="6">
+      <c r="A2" s="2">
         <v>0.227835051546391</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="2">
         <v>0.692307692307692</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -1038,10 +1535,10 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="6">
+      <c r="A3" s="2">
         <v>0.396391752577319</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="2">
         <v>0.178461538461538</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1052,10 +1549,10 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="6">
+      <c r="A4" s="2">
         <v>0.523195876288659</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="2">
         <v>0.107692307692307</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -1066,10 +1563,10 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="6">
+      <c r="A5" s="2">
         <v>0.348453608247422</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="2">
         <v>0.701538461538461</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -1080,10 +1577,10 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="6">
+      <c r="A6" s="2">
         <v>0.547938144329897</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="2">
         <v>0.206153846153845</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -1094,10 +1591,10 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="6">
+      <c r="A7" s="2">
         <v>0.747422680412371</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="2">
         <v>0.153846153846153</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -1108,10 +1605,10 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="6">
+      <c r="A8" s="2">
         <v>0.498453608247422</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="2">
         <v>0.747692307692307</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -1122,10 +1619,10 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="6">
+      <c r="A9" s="2">
         <v>0.648453608247422</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="2">
         <v>0.692307692307692</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -1136,10 +1633,10 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="6">
+      <c r="A10" s="2">
         <v>0.798453608247422</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="2">
         <v>0.612307692307692</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -1168,7 +1665,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1179,10 +1676,10 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="6">
+      <c r="A2" s="2">
         <v>0.232142857142857</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="2">
         <v>-0.687248322147651</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -1193,10 +1690,10 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="6">
+      <c r="A3" s="2">
         <v>0.402232142857142</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="2">
         <v>-0.636241610738255</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1207,10 +1704,10 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="6">
+      <c r="A4" s="2">
         <v>0.528125</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="2">
         <v>-0.657718120805369</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -1221,10 +1718,10 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="6">
+      <c r="A5" s="2">
         <v>0.351339285714285</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="2">
         <v>-0.65503355704698</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -1235,10 +1732,10 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="6">
+      <c r="A6" s="2">
         <v>0.55625</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="2">
         <v>-0.668456375838926</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -1249,10 +1746,10 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="6">
+      <c r="A7" s="2">
         <v>0.754464285714285</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="2">
         <v>-0.748993288590604</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -1263,10 +1760,10 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="6">
+      <c r="A8" s="2">
         <v>0.498660714285714</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="2">
         <v>-0.657718120805369</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -1277,10 +1774,10 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="6">
+      <c r="A9" s="2">
         <v>0.65</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="2">
         <v>-0.695302013422818</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -1291,10 +1788,10 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="6">
+      <c r="A10" s="2">
         <v>0.801339285714285</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="2">
         <v>-0.719463087248322</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -1323,7 +1820,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1334,10 +1831,10 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="6">
+      <c r="A2" s="2">
         <v>0.228643216080401</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="2">
         <v>-0.287878787878787</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -1348,10 +1845,10 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="6">
+      <c r="A3" s="2">
         <v>0.400502512562814</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="2">
         <v>-0.284848484848484</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1362,10 +1859,10 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="6">
+      <c r="A4" s="2">
         <v>0.528643216080402</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="2">
         <v>-0.3</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -1376,10 +1873,10 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="6">
+      <c r="A5" s="2">
         <v>0.349246231155778</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="2">
         <v>-0.278787878787878</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -1390,10 +1887,10 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="6">
+      <c r="A6" s="2">
         <v>0.560301507537688</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="2">
         <v>-0.309090909090909</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -1404,10 +1901,10 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="6">
+      <c r="A7" s="2">
         <v>0.748743718592964</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="2">
         <v>-0.369696969696969</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -1418,10 +1915,10 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="6">
+      <c r="A8" s="2">
         <v>0.498492462311557</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="2">
         <v>-0.296969696969697</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -1432,10 +1929,10 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="6">
+      <c r="A9" s="2">
         <v>0.646231155778894</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="2">
         <v>-0.33030303030303</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -1446,10 +1943,10 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="6">
+      <c r="A10" s="2">
         <v>0.8</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="2">
         <v>-0.393939393939393</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -1478,7 +1975,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1489,10 +1986,10 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="6">
+      <c r="A2" s="2">
         <v>0.233082706766917</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="2">
         <v>-0.804528301886792</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -1503,10 +2000,10 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="6">
+      <c r="A3" s="2">
         <v>0.398496240601503</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="2">
         <v>-0.810566037735849</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1517,10 +2014,10 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="6">
+      <c r="A4" s="2">
         <v>0.526315789473684</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="2">
         <v>-0.819622641509434</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -1531,10 +2028,10 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="6">
+      <c r="A5" s="2">
         <v>0.35187969924812</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="2">
         <v>-0.813584905660377</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -1545,10 +2042,10 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="6">
+      <c r="A6" s="2">
         <v>0.550375939849624</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="2">
         <v>-0.831698113207547</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -1559,10 +2056,10 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="6">
+      <c r="A7" s="2">
         <v>0.750375939849624</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="2">
         <v>-0.922264150943396</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -1573,10 +2070,10 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="6">
+      <c r="A8" s="2">
         <v>0.499248120300751</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="2">
         <v>-0.819622641509434</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -1587,10 +2084,10 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="6">
+      <c r="A9" s="2">
         <v>0.654135338345864</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="2">
         <v>-0.858867924528301</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -1601,13 +2098,168 @@
       </c>
     </row>
     <row r="10">
+      <c r="A10" s="2">
+        <v>0.796992481203007</v>
+      </c>
+      <c r="B10" s="2">
+        <v>-0.928301886792452</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="1">
+        <v>10.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="6">
+        <v>0.231353919239905</v>
+      </c>
+      <c r="B2" s="2">
+        <v>-5.75539568345329E-4</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6">
+        <v>0.402375296912114</v>
+      </c>
+      <c r="B3" s="2">
+        <v>-2.87769784172664E-4</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="6">
+        <v>0.527790973871734</v>
+      </c>
+      <c r="B4" s="2">
+        <v>-2.87769784172664E-4</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="6">
+        <v>0.351068883610451</v>
+      </c>
+      <c r="B5" s="2">
+        <v>-8.63309352517993E-4</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="6">
+        <v>0.553444180522565</v>
+      </c>
+      <c r="B6" s="2">
+        <v>-2.87769784172664E-4</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="6">
+        <v>0.751543942992874</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.0310791366906474</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="6">
+        <v>0.497862232779097</v>
+      </c>
+      <c r="B8" s="2">
+        <v>-2.87769784172664E-4</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="1">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="6">
+        <v>0.650356294536817</v>
+      </c>
+      <c r="B9" s="2">
+        <v>-2.87769784172664E-4</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="1">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="10">
       <c r="A10" s="6">
-        <v>0.796992481203007</v>
-      </c>
-      <c r="B10" s="6">
-        <v>-0.928301886792452</v>
-      </c>
-      <c r="C10" s="1" t="s">
+        <v>0.802850356294537</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.0497841726618705</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="1">

</xml_diff>